<commit_message>
data set - ACER
</commit_message>
<xml_diff>
--- a/fypDS.xlsx
+++ b/fypDS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6F8167-8C18-4000-A4CA-ABB2D38E2922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D07A0D-575C-4290-B759-1123EB79B6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6959E88D-E4AE-4485-A512-4E79A32FE670}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11355" xr2:uid="{6959E88D-E4AE-4485-A512-4E79A32FE670}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="174">
   <si>
     <t>hate</t>
   </si>
@@ -403,6 +403,162 @@
   </si>
   <si>
     <t>Bika ashen den ata deka thalaaganna yanna hadannee.. anee hondai..</t>
+  </si>
+  <si>
+    <t>Puluwanda mata meka budu bana padayak sinduwa dala hdala denda</t>
+  </si>
+  <si>
+    <t>Gelpena aya hamuwenwa eka loke sobawa</t>
+  </si>
+  <si>
+    <t>Vinasai wuththo vinasayi</t>
+  </si>
+  <si>
+    <t>wuththo</t>
+  </si>
+  <si>
+    <t>Dinakshie thamai hodatama kare</t>
+  </si>
+  <si>
+    <t>Donigen athwela idpn http</t>
+  </si>
+  <si>
+    <t>oya baya wenna epa lassana lamayo mata puluwan oyage duka ahanna</t>
+  </si>
+  <si>
+    <t>dasun hodata score karaddi Banuka wage patta kammali pacayala danawa bat karanna enawa witharai.jeewitheta feilding karanna enne ne.kammali pagaya</t>
+  </si>
+  <si>
+    <t>pacayala</t>
+  </si>
+  <si>
+    <t>Dasun shanaka hoda captain kenek. Eth eya eliyen thibba eka hodai. Eya betek vidihata isthawara wela enna ona.</t>
+  </si>
+  <si>
+    <t>Ko huththo dasun</t>
+  </si>
+  <si>
+    <t>huththo</t>
+  </si>
+  <si>
+    <t>SUDUSSATA SUDUSU THANA DENNA KIHOMATH MUNTA OONA UNTA KADE YANA UNGE WARADI WAHANA UNWA MUN BAYAI DASUNTA</t>
+  </si>
+  <si>
+    <t>Wiyali kalapa dason lonthayage cricket iwri</t>
+  </si>
+  <si>
+    <t>Mamanam oyala dennatama godak kamathi adarei</t>
+  </si>
+  <si>
+    <t>Dukai me jeevithe prasidda aprasidda siyalu weda karana gehenun mara kattak kanne hemadema daragena</t>
+  </si>
+  <si>
+    <t>Meyalage vekara oitawada duk vidina minissu kochchara ennawada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kochchara mahansiyak danunath man asama job eka , mokada mage hineth ekama nisa venna athi babalage wada karan pandara nagitala, script mathaka thiyagena, kenek dialogue ekak hari waradduwoth eka sarin sare karala , samaharak vita e waraddana eka auve , wathure ganna shot ekak venna puluwn , kohoma hari shooting iwara venna ra jameta ethakan idala gedara avilla gedara wadath karala nindata yana me job ekath hithana tharam lesi na </t>
+  </si>
+  <si>
+    <t>Moda geniyek.. ratata kelawenakan balan inne meki nam.. vedio eka dekkama appiriya una eththatama.. munta ona thamange eka raja karagena sepa widinna.. kawuruhari wetila thiyana rata godagannawata meki kemathi ne.</t>
+  </si>
+  <si>
+    <t>Puca cududa</t>
+  </si>
+  <si>
+    <t>palayan huttiye yanna</t>
+  </si>
+  <si>
+    <t>huttiye</t>
+  </si>
+  <si>
+    <t>Wada wela yanna ona thadi jiwitha mewa</t>
+  </si>
+  <si>
+    <t>Mun niliyoda hora kana un kamathi hora kana unta ne kuhaka kama moone penawa ugath kamak na ekai ethana penne gon harak ganiyek mun me duppath eka wenuwen newei ktha karanne thamnge malla purawaganna go wetta pasi hamaniyan sajiya ekka</t>
+  </si>
+  <si>
+    <t>wetta pasi</t>
+  </si>
+  <si>
+    <t>hamaniyan</t>
+  </si>
+  <si>
+    <t>Sahodari...Balagena inna...janatha mathayata garu karanna igena ganna...rata hadanna isella…</t>
+  </si>
+  <si>
+    <t>Gon baduwak</t>
+  </si>
+  <si>
+    <t>baduwak</t>
+  </si>
+  <si>
+    <t>Wesa balli...ubata hena respect kara essara...hora ganiyek no tho…</t>
+  </si>
+  <si>
+    <t>wesa</t>
+  </si>
+  <si>
+    <t>balli</t>
+  </si>
+  <si>
+    <t>Oita wada hodai redda ussan pare giyanan</t>
+  </si>
+  <si>
+    <t>Ubata trackda yko. Eka welawaka ekak kynw. Thawa welawaka thawa ekak kiynwa</t>
+  </si>
+  <si>
+    <t>Ko utto kollonata mkuth denne na ne sibaaa</t>
+  </si>
+  <si>
+    <t>utto</t>
+  </si>
+  <si>
+    <t>Tw aluth wuttek awilla</t>
+  </si>
+  <si>
+    <t>wuttek</t>
+  </si>
+  <si>
+    <t>Hemoma inne kibalane utto kollekta dipllko uge satuta blnna</t>
+  </si>
+  <si>
+    <t>kibalane</t>
+  </si>
+  <si>
+    <t>Pissu neda Mokek Hari karanawa dekkama okkoma paddo tika oka karanawa pare yana minissunta Hari karadarayak mun</t>
+  </si>
+  <si>
+    <t>Thopita pissuda pako.gon athal hutho</t>
+  </si>
+  <si>
+    <t>hutho</t>
+  </si>
+  <si>
+    <t>Mewa baladdi mat hemadama edenawa mokada mat aiya keneki nethi nisa</t>
+  </si>
+  <si>
+    <t>Vatun neme podiwttiye ud damm kiypn</t>
+  </si>
+  <si>
+    <t>podiwttiye</t>
+  </si>
+  <si>
+    <t>Me nil wetalau palayak thiyenawa magawa meka pochchiyaka hadanna barid.</t>
+  </si>
+  <si>
+    <t>2000n passe besikayo</t>
+  </si>
+  <si>
+    <t>besikayo</t>
+  </si>
+  <si>
+    <t>Koheda meka thiyenne..matath meya ekka join wenna puluwanda</t>
+  </si>
+  <si>
+    <t>Kavru monca kivat oya yana gamana yanna daruvo taman kamatide tamanta karanna puluvan</t>
+  </si>
+  <si>
+    <t>Pirunu kale diyanosele</t>
   </si>
 </sst>
 </file>
@@ -784,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD71A72-8387-4123-B42C-650C0C79B145}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,7 +2449,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
@@ -2306,9 +2462,11 @@
       <c r="D81">
         <v>0</v>
       </c>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E81" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>0</v>
       </c>
@@ -2321,24 +2479,31 @@
       <c r="D82">
         <v>0</v>
       </c>
-      <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E82" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F83" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -2351,22 +2516,31 @@
       <c r="D84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F85" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0</v>
       </c>
@@ -2379,22 +2553,34 @@
       <c r="D86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F87" t="s">
+        <v>130</v>
+      </c>
+      <c r="G87" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>0</v>
       </c>
@@ -2407,24 +2593,33 @@
       <c r="D88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F89" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -2433,12 +2628,15 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -2447,10 +2645,13 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0</v>
       </c>
@@ -2463,8 +2664,11 @@
       <c r="D92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
@@ -2477,10 +2681,13 @@
       <c r="D93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -2489,10 +2696,13 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0</v>
       </c>
@@ -2505,10 +2715,13 @@
       <c r="D95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -2517,40 +2730,55 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>0</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F97" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F98" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -2559,20 +2787,396 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F100" t="s">
+        <v>146</v>
+      </c>
+      <c r="G100" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>149</v>
+      </c>
+      <c r="F102" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F103" t="s">
+        <v>152</v>
+      </c>
+      <c r="G103" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>0</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>0</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F106" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>0</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F107" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>0</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F108" t="s">
+        <v>161</v>
+      </c>
+      <c r="G108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F110" t="s">
+        <v>43</v>
+      </c>
+      <c r="G110" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>0</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F112" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F114" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>0</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>0</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>0</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>0</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>0</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
         <v>0</v>
       </c>
     </row>

</xml_diff>